<commit_message>
Emission/Demand Data; Delete Redundant Temoatools
</commit_message>
<xml_diff>
--- a/projects/virginia/data/data_virginia.xlsx
+++ b/projects/virginia/data/data_virginia.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10914"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1962D0EC-C419-BD4A-B720-9D65EB8ADA86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EDE16A-7A8E-CA45-949E-8C8B3043FFD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="941" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="941" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2104" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="250">
   <si>
     <t>connection</t>
   </si>
@@ -775,6 +775,18 @@
   </si>
   <si>
     <t>EX_WOOD</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>kton</t>
+  </si>
+  <si>
+    <t>EC_WIND    </t>
+  </si>
+  <si>
+    <t>ED_SOLPV   </t>
   </si>
 </sst>
 </file>
@@ -785,7 +797,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -822,6 +834,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -856,7 +874,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -882,6 +900,7 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10799,8 +10818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10880,40 +10899,88 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
+      <c r="A6" s="15">
+        <v>2030</v>
+      </c>
+      <c r="B6" s="15">
+        <v>509.7</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="15">
+        <v>152.91</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
+      <c r="A7" s="15">
+        <v>2035</v>
+      </c>
+      <c r="B7" s="15">
+        <v>564.79999999999995</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="15">
+        <v>169.44</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="A8" s="15">
+        <v>2040</v>
+      </c>
+      <c r="B8" s="15">
+        <v>616.79999999999995</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="15">
+        <v>400.92</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="A9" s="15">
+        <v>2045</v>
+      </c>
+      <c r="B9" s="15">
+        <v>668.8</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="15">
+        <v>434.72</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
+      <c r="A10" s="15">
+        <v>2050</v>
+      </c>
+      <c r="B10" s="15">
+        <v>720.8</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="15">
+        <v>720.8</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
+      <c r="A11" s="15">
+        <v>2055</v>
+      </c>
+      <c r="B11" s="15">
+        <v>772.7</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="15">
+        <v>772.7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11070,10 +11137,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCEDF73-15BA-AB46-9BE9-827A810B084A}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11162,6 +11229,342 @@
         <v>166</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="15">
+        <v>2025</v>
+      </c>
+      <c r="C7" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" s="15">
+        <v>2025</v>
+      </c>
+      <c r="C8" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="B9" s="15">
+        <v>2025</v>
+      </c>
+      <c r="C9" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="15">
+        <v>2025</v>
+      </c>
+      <c r="C10" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="15">
+        <v>2030</v>
+      </c>
+      <c r="C11" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12" s="15">
+        <v>2030</v>
+      </c>
+      <c r="C12" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13" s="15">
+        <v>2030</v>
+      </c>
+      <c r="C13" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="15">
+        <v>2030</v>
+      </c>
+      <c r="C14" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="15">
+        <v>2035</v>
+      </c>
+      <c r="C15" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="B16" s="15">
+        <v>2035</v>
+      </c>
+      <c r="C16" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="B17" s="15">
+        <v>2035</v>
+      </c>
+      <c r="C17" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="15">
+        <v>2035</v>
+      </c>
+      <c r="C18" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="15">
+        <v>2040</v>
+      </c>
+      <c r="C19" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="B20" s="15">
+        <v>2040</v>
+      </c>
+      <c r="C20" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="B21" s="15">
+        <v>2040</v>
+      </c>
+      <c r="C21" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="15">
+        <v>2040</v>
+      </c>
+      <c r="C22" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="15">
+        <v>2045</v>
+      </c>
+      <c r="C23" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="B24" s="15">
+        <v>2045</v>
+      </c>
+      <c r="C24" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="B25" s="15">
+        <v>2045</v>
+      </c>
+      <c r="C25" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="15">
+        <v>2045</v>
+      </c>
+      <c r="C26" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="15">
+        <v>2050</v>
+      </c>
+      <c r="C27" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="B28" s="15">
+        <v>2050</v>
+      </c>
+      <c r="C28" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="B29" s="15">
+        <v>2050</v>
+      </c>
+      <c r="C29" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="15">
+        <v>2050</v>
+      </c>
+      <c r="C30" s="15">
+        <v>0.08</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11169,7 +11572,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EF032A-2D29-654E-94C4-B44BF2439BC1}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:D8"/>
@@ -11211,6 +11614,90 @@
         <v>240</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="25">
+        <v>2025</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="25">
+        <v>23800</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="25">
+        <v>2030</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4" s="25">
+        <v>19600</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="25">
+        <v>2035</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" s="25">
+        <v>14700</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="25">
+        <v>2040</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="C6" s="25">
+        <v>9800</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="25">
+        <v>2045</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="25">
+        <v>4900</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="25">
+        <v>2050</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8" s="25">
+        <v>0</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>247</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
fixed virginia data discount rate format issues
</commit_message>
<xml_diff>
--- a/projects/virginia/data/data_virginia.xlsx
+++ b/projects/virginia/data/data_virginia.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10914"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EDE16A-7A8E-CA45-949E-8C8B3043FFD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C001104C-F323-AA4B-9EF1-E58A3AEF3B13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="941" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2170" uniqueCount="248">
   <si>
     <t>connection</t>
   </si>
@@ -781,12 +781,6 @@
   </si>
   <si>
     <t>kton</t>
-  </si>
-  <si>
-    <t>EC_WIND    </t>
-  </si>
-  <si>
-    <t>ED_SOLPV   </t>
   </si>
 </sst>
 </file>
@@ -11140,7 +11134,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D30"/>
+      <selection activeCell="D3" sqref="D3:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11230,338 +11224,338 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" t="s">
         <v>119</v>
       </c>
       <c r="B7" s="15">
         <v>2025</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7">
         <v>0.08</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
-        <v>248</v>
+      <c r="A8" t="s">
+        <v>230</v>
       </c>
       <c r="B8" s="15">
         <v>2025</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8">
         <v>0.08</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>249</v>
+      <c r="A9" t="s">
+        <v>231</v>
       </c>
       <c r="B9" s="15">
         <v>2025</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9">
         <v>0.08</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" t="s">
         <v>133</v>
       </c>
       <c r="B10" s="15">
         <v>2025</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10">
         <v>0.08</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" t="s">
         <v>119</v>
       </c>
       <c r="B11" s="15">
         <v>2030</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11">
         <v>0.08</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
-        <v>248</v>
+      <c r="A12" t="s">
+        <v>230</v>
       </c>
       <c r="B12" s="15">
         <v>2030</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12">
         <v>0.08</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
-        <v>249</v>
+      <c r="A13" t="s">
+        <v>231</v>
       </c>
       <c r="B13" s="15">
         <v>2030</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13">
         <v>0.08</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" t="s">
         <v>133</v>
       </c>
       <c r="B14" s="15">
         <v>2030</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14">
         <v>0.08</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" t="s">
         <v>119</v>
       </c>
       <c r="B15" s="15">
         <v>2035</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15">
         <v>0.08</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
-        <v>248</v>
+      <c r="A16" t="s">
+        <v>230</v>
       </c>
       <c r="B16" s="15">
         <v>2035</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16">
         <v>0.08</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
-        <v>249</v>
+      <c r="A17" t="s">
+        <v>231</v>
       </c>
       <c r="B17" s="15">
         <v>2035</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17">
         <v>0.08</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
+      <c r="A18" t="s">
         <v>133</v>
       </c>
       <c r="B18" s="15">
         <v>2035</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18">
         <v>0.08</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
+      <c r="A19" t="s">
         <v>119</v>
       </c>
       <c r="B19" s="15">
         <v>2040</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19">
         <v>0.08</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
-        <v>248</v>
+      <c r="A20" t="s">
+        <v>230</v>
       </c>
       <c r="B20" s="15">
         <v>2040</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20">
         <v>0.08</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
-        <v>249</v>
+      <c r="A21" t="s">
+        <v>231</v>
       </c>
       <c r="B21" s="15">
         <v>2040</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21">
         <v>0.08</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
+      <c r="A22" t="s">
         <v>133</v>
       </c>
       <c r="B22" s="15">
         <v>2040</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22">
         <v>0.08</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
+      <c r="A23" t="s">
         <v>119</v>
       </c>
       <c r="B23" s="15">
         <v>2045</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23">
         <v>0.08</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
-        <v>248</v>
+      <c r="A24" t="s">
+        <v>230</v>
       </c>
       <c r="B24" s="15">
         <v>2045</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24">
         <v>0.08</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
-        <v>249</v>
+      <c r="A25" t="s">
+        <v>231</v>
       </c>
       <c r="B25" s="15">
         <v>2045</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25">
         <v>0.08</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
+      <c r="A26" t="s">
         <v>133</v>
       </c>
       <c r="B26" s="15">
         <v>2045</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26">
         <v>0.08</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="15" t="s">
+      <c r="A27" t="s">
         <v>119</v>
       </c>
       <c r="B27" s="15">
         <v>2050</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27">
         <v>0.08</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
-        <v>248</v>
+      <c r="A28" t="s">
+        <v>230</v>
       </c>
       <c r="B28" s="15">
         <v>2050</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28">
         <v>0.08</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="15" t="s">
-        <v>249</v>
+      <c r="A29" t="s">
+        <v>231</v>
       </c>
       <c r="B29" s="15">
         <v>2050</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29">
         <v>0.08</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="15" t="s">
+      <c r="A30" t="s">
         <v>133</v>
       </c>
       <c r="B30" s="15">
         <v>2050</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30">
         <v>0.08</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>